<commit_message>
Refactor styles and scripts for improved layout and analytics dashboard
- Updated CSS styles for sidebar and header responsiveness.
- Removed unused JavaScript files related to layout management.
- Enhanced sidebar toggle functionality for better user experience.
- Improved toast notifications.
</commit_message>
<xml_diff>
--- a/data/dist.xlsx
+++ b/data/dist.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\invotyx\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE639F9-0056-4BF4-BCC5-11BFC6D789A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F139BC-9530-4E33-B0E8-37E3A4D3E86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Anaesthesia" sheetId="1" r:id="rId1"/>
-    <sheet name="Gynae Obs" sheetId="2" r:id="rId2"/>
-    <sheet name="Medicine" sheetId="3" r:id="rId3"/>
+    <sheet name="Anesthesia" sheetId="1" r:id="rId1"/>
+    <sheet name="Gynae and OBS" sheetId="2" r:id="rId2"/>
+    <sheet name="Medicine and Allied" sheetId="3" r:id="rId3"/>
     <sheet name="Radiology" sheetId="4" r:id="rId4"/>
-    <sheet name="Surgery" sheetId="5" r:id="rId5"/>
+    <sheet name="Surgery and Allied" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -173,9 +173,6 @@
     <t>renal physiology</t>
   </si>
   <si>
-    <t>haemodynamics</t>
-  </si>
-  <si>
     <t>cns physiology</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>musculoskeletal pathology</t>
+  </si>
+  <si>
+    <t>hemodynamics</t>
   </si>
 </sst>
 </file>
@@ -556,11 +556,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1340,7 +1343,7 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -1357,7 +1360,7 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -1378,9 +1381,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1472,7 +1484,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>12</v>
@@ -1483,7 +1495,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1754,10 +1766,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29">
         <v>9</v>
@@ -2199,7 +2211,7 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2213,10 +2225,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C56">
         <v>12</v>
@@ -2237,9 +2249,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2342,7 +2363,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -2353,7 +2374,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -2602,10 +2623,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -2707,7 +2728,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -2911,7 +2932,7 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46">
         <v>4</v>
@@ -3064,7 +3085,7 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C55">
         <v>4</v>
@@ -3081,7 +3102,7 @@
         <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -3095,10 +3116,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57">
         <v>4</v>
@@ -3119,9 +3140,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3235,7 +3265,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -3572,7 +3602,7 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3776,7 +3806,7 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45">
         <v>3</v>
@@ -3912,7 +3942,7 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -3963,7 +3993,7 @@
         <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -3977,10 +4007,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57">
         <v>4</v>
@@ -4001,9 +4031,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -4106,7 +4145,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -4117,7 +4156,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -4366,10 +4405,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -4420,7 +4459,7 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -4624,7 +4663,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43">
         <v>4</v>
@@ -4760,7 +4799,7 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C51">
         <v>7</v>
@@ -4828,7 +4867,7 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C55">
         <v>2</v>
@@ -4842,10 +4881,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C56">
         <v>3</v>

</xml_diff>